<commit_message>
database moved to host
</commit_message>
<xml_diff>
--- a/mymarks.xlsx
+++ b/mymarks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Till Lindeman</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>2022-12-08</t>
+  </si>
+  <si>
+    <t>2022-12-10</t>
   </si>
   <si>
     <t>Geometry</t>
@@ -86,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,10 +119,13 @@
       <c r="F2" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="G2" t="s" s="0">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>2.0</v>
@@ -130,10 +136,13 @@
       <c r="E3" t="n" s="0">
         <v>2.0</v>
       </c>
+      <c r="G3" t="n" s="0">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n" s="0">
         <v>4.0</v>
@@ -144,7 +153,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>5.0</v>

</xml_diff>